<commit_message>
Working on python with spotify
</commit_message>
<xml_diff>
--- a/Spotify/Decades/Lingua_Franca_by_decade.xlsx
+++ b/Spotify/Decades/Lingua_Franca_by_decade.xlsx
@@ -668,7 +668,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,6 +1050,31 @@
       <c r="E15" t="inlineStr">
         <is>
           <t>spotify:track:1TWqyHC7tt4ba3AXOmZoEt</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>La vereda de la puerta de atrás</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Extremoduro</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Yo, Minoría Absoluta</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2002</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>spotify:track:4kJP8Z888wREJ8bRMWNMuk</t>
         </is>
       </c>
     </row>

</xml_diff>